<commit_message>
add functions for combining pft heuristics revise and comment code
</commit_message>
<xml_diff>
--- a/speciesMappingExampleLists/102ae489-04e3-481d-97df-45905837dc1a_Species__FamilyGBIF.xlsx
+++ b/speciesMappingExampleLists/102ae489-04e3-481d-97df-45905837dc1a_Species__FamilyGBIF.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B229"/>
+  <dimension ref="A1:B220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,26 +441,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Family (GBIF)</t>
+          <t>Family GBIF</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Acer campestre</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sapindaceae</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Acer negundo</t>
+          <t>Acer</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +468,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Acer platanoides</t>
+          <t>Acer campestre</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +480,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Acer pseudoplatanus</t>
+          <t>Acer negundo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +492,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Acer platanoides</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,55 +504,55 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Achillea millefolium</t>
+          <t>Acer pseudoplatanus</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Sapindaceae</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Agrimonia eupatoria</t>
+          <t>Achillea millefolium</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Agrostis capillaris</t>
+          <t>Agrimonia eupatoria</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Allium</t>
+          <t>Agrostis capillaris</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Amaryllidaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Allium vineale</t>
+          <t>Allium</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,24 +564,24 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Alopecurus pratensis</t>
+          <t>Allium vineale</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Amaryllidaceae</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Lysimachia arvensis</t>
+          <t>Alopecurus pratensis</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Primulaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
@@ -712,79 +708,79 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Bellis perennis</t>
+          <t>Avenula pubescens</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Betonica officinalis</t>
+          <t>Bellis perennis</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Lamiaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Betula</t>
+          <t>Betonica officinalis</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Betulaceae</t>
+          <t>Lamiaceae</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Borago officinalis</t>
+          <t>Betula</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Boraginaceae</t>
+          <t>Betulaceae</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Brachypodium pinnatum</t>
+          <t>Borago officinalis</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Boraginaceae</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Brassica napus</t>
+          <t>Brachypodium pinnatum</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Brassicaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Brassica oleracea</t>
+          <t>Brassica napus</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -796,7 +792,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Brassicaceae</t>
+          <t>Brassica oleracea</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -808,19 +804,19 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Bromus erectus</t>
+          <t>Brassicaceae</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Brassicaceae</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bromus hordeaceus</t>
+          <t>Bromus erectus</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -832,7 +828,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Bromus sterilis</t>
+          <t>Bromus hordeaceus</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -844,7 +840,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Calamagrostis epigejos</t>
+          <t>Bromus sterilis</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -856,19 +852,19 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Campanula patula</t>
+          <t>Calamagrostis epigejos</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Campanulaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Campanula rapunculoides</t>
+          <t>Campanula patula</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -880,7 +876,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Campanula rotundifolia</t>
+          <t>Campanula rapunculoides</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -892,31 +888,31 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Capsella bursa-pastoris</t>
+          <t>Campanula rotundifolia</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Brassicaceae</t>
+          <t>Campanulaceae</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Carduus acanthoides</t>
+          <t>Capsella bursa-pastoris</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Brassicaceae</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Carduus crispus</t>
+          <t>Carduus acanthoides</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -928,31 +924,31 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Carum carvi</t>
+          <t>Carduus crispus</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Apiaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Centaurea jacea</t>
+          <t>Carum carvi</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Apiaceae</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Centaurea scabiosa</t>
+          <t>Centaurea jacea</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -964,19 +960,19 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Cerastium glomeratum</t>
+          <t>Centaurea scabiosa</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Caryophyllaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Cerastium holosteoides</t>
+          <t>Cerastium glomeratum</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -988,24 +984,24 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Chenopodium album</t>
+          <t>Cerastium holosteoides</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Amaranthaceae</t>
+          <t>Caryophyllaceae</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Chenopodium album</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Amaranthaceae</t>
         </is>
       </c>
     </row>
@@ -1084,24 +1080,24 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Erigeron canadensis</t>
+          <t>Cornus sanguinea</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Cornaceae</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Cornus sanguinea</t>
+          <t>Coronilla varia</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Cornaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
@@ -1216,55 +1212,55 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Elymus repens</t>
+          <t>Draba</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Brassicaceae</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Epilobium tetragonum</t>
+          <t>Elymus repens</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Onagraceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Equisetum arvense</t>
+          <t>Epilobium tetragonum</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Equisetaceae</t>
+          <t>Onagraceae</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Erigeron acris</t>
+          <t>Equisetum arvense</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Equisetaceae</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Erigeron annuus</t>
+          <t>Erigeron acris</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1276,43 +1272,43 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Erodium cicutarium</t>
+          <t>Erigeron annuus</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Geraniaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Draba</t>
+          <t>Erigeron canadensis</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Brassicaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Eryngium campestre</t>
+          <t>Erodium cicutarium</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Apiaceae</t>
+          <t>Geraniaceae</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Falcaria vulgaris</t>
+          <t>Eryngium campestre</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1324,31 +1320,31 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Fallopia convolvulus</t>
+          <t>Falcaria vulgaris</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Polygonaceae</t>
+          <t>Apiaceae</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Fallopia convolvulus</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Polygonaceae</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Festuca ovina</t>
+          <t>Festuca</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1360,7 +1356,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Festuca ovina</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1396,7 +1392,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Festuca</t>
+          <t>Festulolium</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1408,19 +1404,19 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Festulolium</t>
+          <t>Filipendula ulmaria</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Filipendula ulmaria</t>
+          <t>Filipendula vulgaris</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1432,43 +1428,43 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Filipendula vulgaris</t>
+          <t>Fraxinus excelsior</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Oleaceae</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Fraxinus excelsior</t>
+          <t>Fumaria officinalis</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Oleaceae</t>
+          <t>Papaveraceae</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Fumaria officinalis</t>
+          <t>Galium album</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Papaveraceae</t>
+          <t>Rubiaceae</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Galium album</t>
+          <t>Galium aparine</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1480,7 +1476,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Galium aparine</t>
+          <t>Galium mollugo</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1492,7 +1488,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Galium mollugo</t>
+          <t>Galium pomeranicum</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1504,7 +1500,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Galium pomeranicum</t>
+          <t>Galium verum</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1516,12 +1512,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Galium verum</t>
+          <t>Geranium</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Rubiaceae</t>
+          <t>Geraniaceae</t>
         </is>
       </c>
     </row>
@@ -1588,55 +1584,55 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Geranium</t>
+          <t>Geum urbanum</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Geraniaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Geum urbanum</t>
+          <t>Glechoma hederacea</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Lamiaceae</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Glechoma hederacea</t>
+          <t>Helictotrichon pratense</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Lamiaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Helictotrichon pratense</t>
+          <t>Heracleum sphondylium</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Apiaceae</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Avenula pubescens</t>
+          <t>Holcus lanatus</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1648,19 +1644,19 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Heracleum sphondylium</t>
+          <t>Hypericum perforatum</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Apiaceae</t>
+          <t>Hypericaceae</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Pilosella officinarum</t>
+          <t>Hypochaeris radicata</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1672,31 +1668,31 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Holcus lanatus</t>
+          <t>Knautia arvensis</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Caprifoliaceae</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Hypericum perforatum</t>
+          <t>Koeleria macrantha</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Hypericaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Hypochaeris radicata</t>
+          <t>Lactuca serriola</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1708,31 +1704,31 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Knautia arvensis</t>
+          <t>Lamium amplexicaule</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Caprifoliaceae</t>
+          <t>Lamiaceae</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Koeleria macrantha</t>
+          <t>Lamium purpureum</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Lamiaceae</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Lactuca serriola</t>
+          <t>Lapsana communis</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1744,31 +1740,31 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Lamium amplexicaule</t>
+          <t>Lathyrus pratensis</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Lamiaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Lamium purpureum</t>
+          <t>Lathyrus tuberosus</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Lamiaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Lapsana communis</t>
+          <t>Leontodon autumnalis</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1780,123 +1776,127 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Lathyrus pratensis</t>
+          <t>Leontodon hispidus</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Lathyrus tuberosus</t>
+          <t>Leucanthemum vulgare</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Leontodon autumnalis</t>
+          <t>Linaria vulgaris</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Leontodon hispidus</t>
+          <t>Lolium multiflorum</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Leucanthemum vulgare</t>
+          <t>Lolium perenne</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Seseli libanotis</t>
+          <t>Lotus corniculatus</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Apiaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Linaria vulgaris</t>
+          <t>Lotus pedunculatus</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr"/>
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Lysimachia arvensis</t>
+        </is>
+      </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>not found</t>
+          <t>Primulaceae</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Lolium multiflorum</t>
+          <t>Lysimachia nummularia</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Primulaceae</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Lolium perenne</t>
+          <t>Malva sylvestris</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Malvaceae</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Lotus corniculatus</t>
+          <t>Medicago</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -1908,7 +1908,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Lotus pedunculatus</t>
+          <t>Medicago falcata</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -1920,183 +1920,187 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Silene flos-cuculi</t>
+          <t>Medicago lupulina</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Caryophyllaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Lysimachia nummularia</t>
+          <t>Medicago varia</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Primulaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Malva sylvestris</t>
+          <t>Melampyrum pratense</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Malvaceae</t>
+          <t>Orobanchaceae</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Myosotis arvensis</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Boraginaceae</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Medicago falcata</t>
+          <t>Noccaea perfoliata</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Brassicaceae</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Medicago lupulina</t>
+          <t>Papaver rhoeas</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Papaveraceae</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Medicago</t>
+          <t>Pastinaca sativa</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Apiaceae</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Medicago varia</t>
+          <t>Petrorhagia prolifera</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Caryophyllaceae</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Melampyrum pratense</t>
+          <t>Phleum pratense</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Orobanchaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Noccaea perfoliata</t>
+          <t>Picris hieracioides</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Brassicaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr"/>
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Pilosella officinarum</t>
+        </is>
+      </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>not found</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Myosotis arvensis</t>
+          <t>Pimpinella saxifraga</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Boraginaceae</t>
+          <t>Apiaceae</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Papaver rhoeas</t>
+          <t>Plantago lanceolata</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Papaveraceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Pastinaca sativa</t>
+          <t>Plantago major</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Apiaceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Petrorhagia prolifera</t>
+          <t>Plantago media</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Caryophyllaceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Phleum pratense</t>
+          <t>Poa angustifolia</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2108,563 +2112,571 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Picris hieracioides</t>
+          <t>Poa annua</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Pimpinella saxifraga</t>
+          <t>Poa bulbosa</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Apiaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Plantago lanceolata</t>
+          <t>Poa pratensis</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Plantago major</t>
+          <t>Poa trivialis</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Plantago media</t>
+          <t>Poaceae</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Poa angustifolia</t>
+          <t>Polygonum aviculare</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Polygonaceae</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Poa annua</t>
+          <t>Populus canadensis</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Salicaceae</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Poa bulbosa</t>
+          <t>Potentilla argentea</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Poa pratensis</t>
+          <t>Poterium sanguisorba</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Poa trivialis</t>
+          <t>Prunella vulgaris</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Lamiaceae</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Prunus</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Polygonum aviculare</t>
+          <t>Prunus avium</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Polygonaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Populus canadensis</t>
+          <t>Prunus mahaleb</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Salicaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Potentilla argentea</t>
+          <t>Ranunculus acris</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Ranunculaceae</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Prunella vulgaris</t>
+          <t>Ranunculus auricomus</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Lamiaceae</t>
+          <t>Ranunculaceae</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Prunus avium</t>
+          <t>Ranunculus bulbosus</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Ranunculaceae</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Prunus mahaleb</t>
+          <t>Ranunculus repens</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Ranunculaceae</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Prunus</t>
+          <t>Rhinanthus minor</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Orobanchaceae</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Ranunculus acris</t>
+          <t>Rubus</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Ranunculaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Ranunculus auricomus</t>
+          <t>Rubus caesius</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Ranunculaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Ranunculus bulbosus</t>
+          <t>Rubus idaeus</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Ranunculaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Ranunculus repens</t>
+          <t>Rumex crispus</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Ranunculaceae</t>
+          <t>Polygonaceae</t>
         </is>
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr"/>
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Salvia pratensis</t>
+        </is>
+      </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>not found</t>
+          <t>Lamiaceae</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Rhinanthus minor</t>
+          <t>Sambucus nigra</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Orobanchaceae</t>
+          <t>Viburnaceae</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Rubus caesius</t>
+          <t>Saxifraga granulata</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Saxifragaceae</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Rubus idaeus</t>
+          <t>Scabiosa ochroleuca</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Caprifoliaceae</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Rubus</t>
+          <t>Senecio</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Rumex crispus</t>
+          <t>Senecio jacobaea</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Polygonaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Salvia pratensis</t>
+          <t>Senecio vernalis</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Lamiaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Sambucus nigra</t>
+          <t>Senecio vulgaris</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Viburnaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Poterium sanguisorba</t>
+          <t>Seseli libanotis</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Apiaceae</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Saxifraga granulata</t>
+          <t>Setaria viridis</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Saxifragaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Scabiosa ochroleuca</t>
+          <t>Silaum silaus</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Caprifoliaceae</t>
+          <t>Apiaceae</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Coronilla varia</t>
+          <t>Silene flos-cuculi</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Caryophyllaceae</t>
         </is>
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr"/>
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Silene latifolia</t>
+        </is>
+      </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>not found</t>
+          <t>Caryophyllaceae</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Senecio jacobaea</t>
+          <t>Silene noctiflora</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Caryophyllaceae</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Senecio</t>
+          <t>Silene nutans</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Caryophyllaceae</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Senecio vernalis</t>
+          <t>Silene vulgaris</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Caryophyllaceae</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Senecio vulgaris</t>
+          <t>Sinapis arvensis</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Brassicaceae</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Setaria viridis</t>
+          <t>Solanum tuberosum</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Solanaceae</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Silaum silaus</t>
+          <t>Solidago canadensis</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Apiaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Silene latifolia</t>
+          <t>Sonchus arvensis</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Caryophyllaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Silene noctiflora</t>
+          <t>Sonchus asper</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Caryophyllaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Silene nutans</t>
+          <t>Sonchus oleraceus</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Caryophyllaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Silene vulgaris</t>
+          <t>Stachys recta</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Caryophyllaceae</t>
+          <t>Lamiaceae</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Sinapis arvensis</t>
+          <t>Stellaria graminea</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Brassicaceae</t>
+          <t>Caryophyllaceae</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Solanum tuberosum</t>
+          <t>Stellaria media</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Solanaceae</t>
+          <t>Caryophyllaceae</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Solidago canadensis</t>
+          <t>Tanacetum vulgare</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -2676,7 +2688,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Sonchus arvensis</t>
+          <t>Taraxacum officinale</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -2688,19 +2700,19 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Sonchus asper</t>
+          <t>Thlaspi arvense</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Brassicaceae</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Sonchus oleraceus</t>
+          <t>Tragopogon dubius</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -2712,103 +2724,103 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Stachys recta</t>
+          <t>Tragopogon orientalis</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Lamiaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Stellaria graminea</t>
+          <t>Tragopogon pratensis</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Caryophyllaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Stellaria media</t>
+          <t>Trifolium arvense</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Caryophyllaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Tanacetum vulgare</t>
+          <t>Trifolium campestre</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Taraxacum officinale</t>
+          <t>Trifolium dubium</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Thlaspi arvense</t>
+          <t>Trifolium hybridum</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Brassicaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Tragopogon dubius</t>
+          <t>Trifolium pratense</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Tragopogon orientalis</t>
+          <t>Trifolium repens</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Tragopogon pratensis</t>
+          <t>Tripleurospermum inodorum</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -2820,344 +2832,240 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Trifolium arvense</t>
+          <t>Trisetum flavescens</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Trifolium campestre</t>
+          <t>Triticum</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Poaceae</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Trifolium dubium</t>
+          <t>Tussilago farfara</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Trifolium hybridum</t>
+          <t>Urtica urens</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Urticaceae</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Trifolium pratense</t>
+          <t>Verbascum lychnitis</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Scrophulariaceae</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Trifolium repens</t>
+          <t>Verbascum thapsus</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Scrophulariaceae</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Tripleurospermum inodorum</t>
+          <t>Veronica agrestis</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Trisetum flavescens</t>
+          <t>Veronica arvensis</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Triticum</t>
+          <t>Veronica chamaedrys</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Tussilago farfara</t>
+          <t>Veronica hederifolia</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Urtica urens</t>
+          <t>Veronica persica</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Urticaceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Verbascum lychnitis</t>
+          <t>Veronica serpyllifolia</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Scrophulariaceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Verbascum thapsus</t>
+          <t>Vicia</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Scrophulariaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Veronica agrestis</t>
+          <t>Vicia cracca</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Veronica arvensis</t>
+          <t>Vicia hirsuta</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Veronica chamaedrys</t>
+          <t>Vicia sativa</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Veronica hederifolia</t>
+          <t>Vicia sepium</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Veronica persica</t>
+          <t>Vicia tetrasperma</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="219">
-      <c r="A219" t="inlineStr"/>
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Vicia villosa</t>
+        </is>
+      </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>not found</t>
+          <t>Fabaceae</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Veronica serpyllifolia</t>
+          <t>Viola arvensis</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
-        </is>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="inlineStr">
-        <is>
-          <t>Vicia</t>
-        </is>
-      </c>
-      <c r="B221" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="inlineStr">
-        <is>
-          <t>Vicia cracca</t>
-        </is>
-      </c>
-      <c r="B222" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="inlineStr">
-        <is>
-          <t>Vicia hirsuta</t>
-        </is>
-      </c>
-      <c r="B223" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="inlineStr">
-        <is>
-          <t>Vicia sativa</t>
-        </is>
-      </c>
-      <c r="B224" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="inlineStr">
-        <is>
-          <t>Vicia sepium</t>
-        </is>
-      </c>
-      <c r="B225" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="inlineStr">
-        <is>
-          <t>Vicia tetrasperma</t>
-        </is>
-      </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="inlineStr">
-        <is>
-          <t>Vicia villosa</t>
-        </is>
-      </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="inlineStr">
-        <is>
-          <t>Viola arvensis</t>
-        </is>
-      </c>
-      <c r="B228" t="inlineStr">
-        <is>
           <t>Violaceae</t>
-        </is>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="inlineStr">
-        <is>
-          <t>Festuca</t>
-        </is>
-      </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t>Poaceae</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
always keep family infos, keep orig names also if not changed by GBIF
</commit_message>
<xml_diff>
--- a/speciesMappingExampleLists/102ae489-04e3-481d-97df-45905837dc1a_Species__FamilyGBIF.xlsx
+++ b/speciesMappingExampleLists/102ae489-04e3-481d-97df-45905837dc1a_Species__FamilyGBIF.xlsx
@@ -456,7 +456,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Acer campestre</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -468,7 +468,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Acer campestre</t>
+          <t>Acer negundo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -480,7 +480,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Acer negundo</t>
+          <t>Acer platanoides</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -492,7 +492,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Acer platanoides</t>
+          <t>Acer pseudoplatanus</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -504,7 +504,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Acer pseudoplatanus</t>
+          <t>Acer species</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -552,7 +552,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Allium</t>
+          <t>Allium species</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Apiaceae</t>
+          <t>Apiaceae species</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -684,7 +684,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Asteraceae species</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -744,7 +744,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Betula</t>
+          <t>Betula species</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Brassicaceae</t>
+          <t>Brassicaceae species</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1212,7 +1212,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Draba</t>
+          <t>Draba species</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1344,7 +1344,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Festuca</t>
+          <t>Festuca ovina</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1356,7 +1356,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Festuca ovina</t>
+          <t>Festuca rubra</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1368,7 +1368,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Festuca rubra</t>
+          <t>Festuca rupicola</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1380,7 +1380,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Festuca rupicola</t>
+          <t>Festuca species</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1512,7 +1512,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Geranium</t>
+          <t>Geranium molle</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1524,7 +1524,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Geranium molle</t>
+          <t>Geranium pratense</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1536,7 +1536,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Geranium pratense</t>
+          <t>Geranium pusillum</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1548,7 +1548,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Geranium pusillum</t>
+          <t>Geranium pyrenaicum</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Geranium pyrenaicum</t>
+          <t>Geranium rotundifolium</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1572,7 +1572,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Geranium rotundifolium</t>
+          <t>Geranium species</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1896,7 +1896,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Medicago</t>
+          <t>Medicago falcata</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -1908,7 +1908,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Medicago falcata</t>
+          <t>Medicago lupulina</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -1920,7 +1920,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Medicago lupulina</t>
+          <t>Medicago species</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -2160,7 +2160,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Poaceae</t>
+          <t>Poaceae species</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -2232,7 +2232,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Prunus</t>
+          <t>Prunus avium</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -2244,7 +2244,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Prunus avium</t>
+          <t>Prunus mahaleb</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -2256,7 +2256,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Prunus mahaleb</t>
+          <t>Prunus species</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -2328,7 +2328,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Rubus</t>
+          <t>Rubus caesius</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -2340,7 +2340,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Rubus caesius</t>
+          <t>Rubus idaeus</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -2352,7 +2352,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Rubus idaeus</t>
+          <t>Rubus species</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -2424,7 +2424,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Senecio</t>
+          <t>Senecio jacobaea</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -2436,7 +2436,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Senecio jacobaea</t>
+          <t>Senecio species</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -2844,7 +2844,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Triticum</t>
+          <t>Triticum species</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -2976,7 +2976,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Vicia</t>
+          <t>Vicia cracca</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -2988,7 +2988,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Vicia cracca</t>
+          <t>Vicia hirsuta</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -3000,7 +3000,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Vicia hirsuta</t>
+          <t>Vicia sativa</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -3012,7 +3012,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Vicia sativa</t>
+          <t>Vicia sepium</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -3024,7 +3024,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Vicia sepium</t>
+          <t>Vicia species</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">

</xml_diff>